<commit_message>
added code for cross browser
</commit_message>
<xml_diff>
--- a/Customers/NextGen/TestSuite1Data.xlsx
+++ b/Customers/NextGen/TestSuite1Data.xlsx
@@ -4,14 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="20040" windowHeight="6225" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="20040" windowHeight="6225" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="TC01" sheetId="2" r:id="rId1"/>
-    <sheet name="TC03" sheetId="6" r:id="rId2"/>
-    <sheet name="TC04" sheetId="7" r:id="rId3"/>
-    <sheet name="TC05" sheetId="4" r:id="rId4"/>
-    <sheet name="TC02" sheetId="8" r:id="rId5"/>
+    <sheet name="TC02" sheetId="8" r:id="rId2"/>
+    <sheet name="TC03" sheetId="6" r:id="rId3"/>
+    <sheet name="TC04" sheetId="9" r:id="rId4"/>
+    <sheet name="TC05" sheetId="10" r:id="rId5"/>
+    <sheet name="TC06" sheetId="11" r:id="rId6"/>
+    <sheet name="TC07" sheetId="12" r:id="rId7"/>
+    <sheet name="TC041" sheetId="7" r:id="rId8"/>
+    <sheet name="TC051" sheetId="4" r:id="rId9"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst>
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="108">
   <si>
     <t>password</t>
   </si>
@@ -91,15 +95,6 @@
     <t>Charges/Payments/Adjustments summary</t>
   </si>
   <si>
-    <t>BillingStatusTitle</t>
-  </si>
-  <si>
-    <t>BillingStatusInfoText</t>
-  </si>
-  <si>
-    <t>Daily billing status</t>
-  </si>
-  <si>
     <t>DailyVisitsBillsTitle</t>
   </si>
   <si>
@@ -121,36 +116,18 @@
     <t>BillingBacklogTitle</t>
   </si>
   <si>
-    <t>Daily billing backlog</t>
-  </si>
-  <si>
     <t>BillingBacklogInfoText</t>
   </si>
   <si>
     <t>Review the billing process preformance. Look for trends above or below average.</t>
   </si>
   <si>
-    <t>DailyUnsignedTitle</t>
-  </si>
-  <si>
-    <t>DailyUnsignedInfoText</t>
-  </si>
-  <si>
-    <t>Daily unsigned</t>
-  </si>
-  <si>
-    <t>Displays various available billing status. Daily backlog (bills to be submitted / resubmitted), bills created( specific day), On hold (due to missing information etc.), pending signoff by provider and bills submitted on a day. Helps manage the backlog. Look for trends above or below average</t>
-  </si>
-  <si>
     <t>Visit represents the patient encounters and bills refers to claims related to visits. Volume trend is key indicator to manage the utilization and billing process productivity. Review the variances to optimize.</t>
   </si>
   <si>
     <t>Average Day difference between Date of Service and Bill Submitted. Review the lag process to drive improvement effort.</t>
   </si>
   <si>
-    <t>Review the process hold up. Follow up if the unsigned bills are increasing above the acceptable level.</t>
-  </si>
-  <si>
     <t>NextGen\Nagendra</t>
   </si>
   <si>
@@ -170,6 +147,213 @@
   </si>
   <si>
     <t>Jordan Valley</t>
+  </si>
+  <si>
+    <t>Daily pending bills</t>
+  </si>
+  <si>
+    <t>Payment % = sum of 6 months payments *100/ (sum of 6 months charges – sum of 6 months not charges)+ sum of 6 months payments. Focus on the variances and identify the root causes by reviewing the CPT counts and A/R related metrics. Higher % is better as it indicates lower A/R and lower rejection of claims.</t>
+  </si>
+  <si>
+    <t>PaymentpercentageInfoText</t>
+  </si>
+  <si>
+    <t>PaymentpercentageTitle</t>
+  </si>
+  <si>
+    <t>Payment %</t>
+  </si>
+  <si>
+    <t>CPARInfoText</t>
+  </si>
+  <si>
+    <t>CPARTitle</t>
+  </si>
+  <si>
+    <t>Charges/Payments/Adjustments/Refunds summary</t>
+  </si>
+  <si>
+    <t>CPTBySpecialityTitle</t>
+  </si>
+  <si>
+    <t>CPTBySpecialityInfoText</t>
+  </si>
+  <si>
+    <t>Procedure codes (CPT) volume by speciality</t>
+  </si>
+  <si>
+    <t>Volume of procedure codes by speciality provides insight to revenue and operations improvement opportunities.</t>
+  </si>
+  <si>
+    <t>ARindaysTitle</t>
+  </si>
+  <si>
+    <t>ARindaysInfoText</t>
+  </si>
+  <si>
+    <t>RollingARTitle</t>
+  </si>
+  <si>
+    <t>RollingARInfoText</t>
+  </si>
+  <si>
+    <t>ARagingTitle</t>
+  </si>
+  <si>
+    <t>ARagingInfoText</t>
+  </si>
+  <si>
+    <t>PaymentlagTitle</t>
+  </si>
+  <si>
+    <t>PaymentlagInfoText</t>
+  </si>
+  <si>
+    <t>Calculates days in A/R as the total A/R, divided by gross charges average of 6 months. Lower A/R days trend is critical for business. Reduction in bill creation lag, submission lag and improvement in claim completness and coding accuracy will help reduce days in A/R.</t>
+  </si>
+  <si>
+    <t>Days in A/R</t>
+  </si>
+  <si>
+    <t>Rolling A/R</t>
+  </si>
+  <si>
+    <t>Amount of A/R in a month is previous months A/R plus charges minus non charges. Reducing A/R amount indicates improved billing process (assuming a business growing). Billing process metrics like bill creation lag, submission lag, claim completeness and coding accuracey will help reduce the amount in A/R</t>
+  </si>
+  <si>
+    <t>A/R aging</t>
+  </si>
+  <si>
+    <t>Days interval includes the charges of unpaid claims from the selected month. Higher A/R in 0-30 days is a good indicator and AR in other intervals need to have process to reduce.</t>
+  </si>
+  <si>
+    <t>Payment lag</t>
+  </si>
+  <si>
+    <t>It is sum of bill Lag (DOS to claim created), submit lag (claim created to claim submitted), approved lag(claim submitted to claim approved), payment lag (claim approved to payment) and post lag(payment to payment posting). Lower lag times are better to reduce A/R. Helps identifying the rootcause for the cycle time variances.</t>
+  </si>
+  <si>
+    <t>DenialsValueandVolumeTitle</t>
+  </si>
+  <si>
+    <t>DenialsValueandVolumeInfoText</t>
+  </si>
+  <si>
+    <t>GrossDenialValueandVolumeTitle</t>
+  </si>
+  <si>
+    <t>GrossDenialValueandVolumeInfoText</t>
+  </si>
+  <si>
+    <t>GrossremittancevalueTitle</t>
+  </si>
+  <si>
+    <t>GrossremittancevalueInfoText</t>
+  </si>
+  <si>
+    <t>GrossremittancevolumeTitle</t>
+  </si>
+  <si>
+    <t>GrossremittancevolumeInfoText</t>
+  </si>
+  <si>
+    <t>Denials value and volume</t>
+  </si>
+  <si>
+    <t>Gross denials value and volume</t>
+  </si>
+  <si>
+    <t>Gross remittance value</t>
+  </si>
+  <si>
+    <t>Gross remittance volume</t>
+  </si>
+  <si>
+    <t>BillssubmittedtopayerTitle</t>
+  </si>
+  <si>
+    <t>BillssubmittedtopayerInfoText</t>
+  </si>
+  <si>
+    <t>CollectionsbypayerTitle</t>
+  </si>
+  <si>
+    <t>CollectionsbypayerInfoText</t>
+  </si>
+  <si>
+    <t>E&amp;MNewTitle</t>
+  </si>
+  <si>
+    <t>E&amp;MNewInfoText</t>
+  </si>
+  <si>
+    <t>E&amp;MEstablishedTitle</t>
+  </si>
+  <si>
+    <t>E&amp;MEstablishedInfoText</t>
+  </si>
+  <si>
+    <t>E&amp;MNewPercentageTitle</t>
+  </si>
+  <si>
+    <t>E&amp;MNewPercentageInfoText</t>
+  </si>
+  <si>
+    <t>E&amp;MExistingPercentageTitle</t>
+  </si>
+  <si>
+    <t>E&amp;MExistingPercentageInfoText</t>
+  </si>
+  <si>
+    <t>BilledVisitsTitle</t>
+  </si>
+  <si>
+    <t>BilledVisitsInfoText</t>
+  </si>
+  <si>
+    <t>Count of bills submitted to the insurance group</t>
+  </si>
+  <si>
+    <t>Bills submitted to payer</t>
+  </si>
+  <si>
+    <t>Collections by payer</t>
+  </si>
+  <si>
+    <t>Sum of payments by top 10 insurance carrier filtered by provider</t>
+  </si>
+  <si>
+    <t>E&amp;M new</t>
+  </si>
+  <si>
+    <t>Evaluation and management (E&amp;M) codes for new patient office or other outpatient visits. Coding erros results in delayed payment, under payment and even audits.</t>
+  </si>
+  <si>
+    <t>E&amp;M established</t>
+  </si>
+  <si>
+    <t>Evaluation and management (E&amp;M) codes for established patient office or other outpatient visits. Coding erros results in delayed payment, under payment and even audits.</t>
+  </si>
+  <si>
+    <t>E&amp;M new %</t>
+  </si>
+  <si>
+    <t>% of evaluation and management (E&amp;M) codes for new patient office or other outpatient visits. Coding erros results in delayed payment, under payment and even audits.</t>
+  </si>
+  <si>
+    <t>E&amp;M established %</t>
+  </si>
+  <si>
+    <t>% of evaluation and management (E&amp;M) codes for established patient office or other outpatient visits. Coding erros results in delayed payment, under payment and even audits.</t>
+  </si>
+  <si>
+    <t>Billed visits by insurance group</t>
+  </si>
+  <si>
+    <t>Provides the payerclass and insurance group volume. This gives an insight to potential revenue stream along with insight to manage payer contracts.</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -226,10 +410,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -561,10 +746,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -577,213 +762,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="36.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" customWidth="1"/>
-    <col min="11" max="11" width="19.7109375" customWidth="1"/>
-    <col min="12" max="12" width="21.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L2" t="s">
-        <v>40</v>
-      </c>
-      <c r="M2">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="65.140625" customWidth="1"/>
-    <col min="4" max="4" width="38.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D1" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -805,7 +787,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>14</v>
@@ -832,21 +814,21 @@
         <v>9</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C2">
         <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -878,16 +860,16 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C3">
         <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
@@ -919,16 +901,16 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C4">
         <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
@@ -956,6 +938,639 @@
       </c>
       <c r="M4">
         <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="35.85546875" customWidth="1"/>
+    <col min="5" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" customWidth="1"/>
+    <col min="8" max="8" width="30" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" customWidth="1"/>
+    <col min="10" max="10" width="27" customWidth="1"/>
+    <col min="11" max="11" width="28.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" customWidth="1"/>
+    <col min="5" max="5" width="32.42578125" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" customWidth="1"/>
+    <col min="7" max="7" width="37" customWidth="1"/>
+    <col min="8" max="8" width="30.140625" customWidth="1"/>
+    <col min="9" max="9" width="30.85546875" customWidth="1"/>
+    <col min="10" max="10" width="29.140625" customWidth="1"/>
+    <col min="11" max="11" width="31.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="J2" t="s">
+        <v>78</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" customWidth="1"/>
+    <col min="7" max="7" width="36.85546875" customWidth="1"/>
+    <col min="8" max="8" width="31.85546875" customWidth="1"/>
+    <col min="9" max="9" width="28.5703125" customWidth="1"/>
+    <col min="10" max="10" width="34.85546875" customWidth="1"/>
+    <col min="11" max="17" width="32.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="J2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="R2">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="65.140625" customWidth="1"/>
+    <col min="4" max="4" width="38.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added saved and applied filter test
</commit_message>
<xml_diff>
--- a/Customers/NextGen/TestSuite1Data.xlsx
+++ b/Customers/NextGen/TestSuite1Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="20040" windowHeight="6225" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="20040" windowHeight="6225" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="TC01" sheetId="2" r:id="rId1"/>
@@ -14,8 +14,12 @@
     <sheet name="TC05" sheetId="10" r:id="rId5"/>
     <sheet name="TC06" sheetId="11" r:id="rId6"/>
     <sheet name="TC07" sheetId="12" r:id="rId7"/>
-    <sheet name="TC041" sheetId="7" r:id="rId8"/>
+    <sheet name="TC08" sheetId="7" r:id="rId8"/>
     <sheet name="TC051" sheetId="4" r:id="rId9"/>
+    <sheet name="TC09" sheetId="14" r:id="rId10"/>
+    <sheet name="TC10" sheetId="15" r:id="rId11"/>
+    <sheet name="TC11" sheetId="16" r:id="rId12"/>
+    <sheet name="TC12" sheetId="17" r:id="rId13"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst>
@@ -30,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="124">
   <si>
     <t>password</t>
   </si>
@@ -354,6 +358,54 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>ChangeStatus</t>
+  </si>
+  <si>
+    <t>password changed successfully</t>
+  </si>
+  <si>
+    <t>NewPassword</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>RunAsLabel</t>
+  </si>
+  <si>
+    <t>aaron.rucker@uthsc.edu</t>
+  </si>
+  <si>
+    <t>CWC\Admin</t>
+  </si>
+  <si>
+    <t>JORDAN\User</t>
+  </si>
+  <si>
+    <t>NotAnumber</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>Practices</t>
+  </si>
+  <si>
+    <t>University Of Tennessee,UT Medical Group, Inc.</t>
+  </si>
+  <si>
+    <t>AppliedFilterTitle</t>
+  </si>
+  <si>
+    <t>SavedFilterTitle</t>
+  </si>
+  <si>
+    <t>Applied Filter</t>
+  </si>
+  <si>
+    <t>Saved Filter</t>
   </si>
 </sst>
 </file>
@@ -760,12 +812,226 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="4" width="30.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="6" width="42.85546875" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="4" width="30.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -773,10 +1039,11 @@
     <col min="1" max="1" width="20.140625" customWidth="1"/>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -790,34 +1057,37 @@
         <v>34</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -831,34 +1101,37 @@
         <v>35</v>
       </c>
       <c r="E2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="G2">
-        <v>10</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" t="s">
-        <v>10</v>
-      </c>
       <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
         <v>11</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>12</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>13</v>
       </c>
-      <c r="M2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="N2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -872,34 +1145,37 @@
         <v>36</v>
       </c>
       <c r="E3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>4</v>
       </c>
-      <c r="G3">
-        <v>10</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
         <v>16</v>
       </c>
-      <c r="I3" t="s">
-        <v>10</v>
-      </c>
       <c r="J3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" t="s">
         <v>11</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>12</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>13</v>
       </c>
-      <c r="M3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="N3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -913,30 +1189,33 @@
         <v>38</v>
       </c>
       <c r="E4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>4</v>
       </c>
-      <c r="G4">
-        <v>10</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
         <v>16</v>
       </c>
-      <c r="I4" t="s">
-        <v>10</v>
-      </c>
       <c r="J4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" t="s">
         <v>11</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>12</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>13</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>10</v>
       </c>
     </row>
@@ -950,7 +1229,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J2"/>
+      <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1484,7 +1763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>